<commit_message>
Sell clock error fixed
</commit_message>
<xml_diff>
--- a/boughtList.xlsx
+++ b/boughtList.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>RI</t>
   </si>
@@ -102,16 +102,7 @@
     <t>08 Nov 2019</t>
   </si>
   <si>
-    <t>ADANI54145</t>
-  </si>
-  <si>
     <t>ITT01</t>
-  </si>
-  <si>
-    <t>11 Nov 2019</t>
-  </si>
-  <si>
-    <t>DT07</t>
   </si>
 </sst>
 </file>
@@ -429,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -454,35 +445,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>72.05</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>87.9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4">
-        <v>2870.77</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removing double API call
</commit_message>
<xml_diff>
--- a/boughtList.xlsx
+++ b/boughtList.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>RI</t>
   </si>
@@ -138,9 +138,6 @@
     <t>03 Jan 2008</t>
   </si>
   <si>
-    <t>04 Jan 2008</t>
-  </si>
-  <si>
     <t>05 Jan 2008</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
   </si>
   <si>
     <t>04 Dec 2019</t>
-  </si>
-  <si>
-    <t>ITD02</t>
   </si>
   <si>
     <t>ICI02</t>
@@ -489,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -512,7 +506,7 @@
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -559,66 +553,66 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>48</v>
+        <v>85.85</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>85.85</v>
+        <v>159.15</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>159.15</v>
+        <v>33.6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>33.6</v>
+        <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>98</v>
+        <v>122.08</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
@@ -629,27 +623,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>122.08</v>
+        <v>46.75</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>46.75</v>
+        <v>147.13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11">
         <v>100</v>
@@ -657,69 +651,69 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>147.13</v>
+        <v>169.49600000000001</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>169.49600000000001</v>
+        <v>277.76</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13">
-        <v>75</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>277.76</v>
+        <v>119.8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14">
-        <v>120</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>119.8</v>
+        <v>19.45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15">
-        <v>74</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>19.45</v>
+        <v>46.5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16">
         <v>100</v>
@@ -727,99 +721,71 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>46.5</v>
+        <v>60.35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D17">
-        <v>100</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>60.35</v>
+        <v>160</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18">
-        <v>56</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>160</v>
+        <v>85.9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B20">
-        <v>85.9</v>
+        <v>210.2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B21">
-        <v>210.2</v>
+        <v>522.79999999999995</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D21">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22">
-        <v>339.3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23">
-        <v>522.79999999999995</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating clock to run at 12 SGT
</commit_message>
<xml_diff>
--- a/boughtList.xlsx
+++ b/boughtList.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>RI</t>
   </si>
@@ -160,12 +160,6 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>GAE</t>
-  </si>
-  <si>
-    <t>29 Jan 2020</t>
-  </si>
-  <si>
     <t>USF</t>
   </si>
   <si>
@@ -176,12 +170,6 @@
   </si>
   <si>
     <t>BA</t>
-  </si>
-  <si>
-    <t>20 Feb 2020</t>
-  </si>
-  <si>
-    <t>CAR</t>
   </si>
 </sst>
 </file>
@@ -499,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -527,71 +515,43 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B2">
-        <v>490.95</v>
+        <v>320.88</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3">
-        <v>320.88</v>
+        <v>55.25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B4">
-        <v>158.1</v>
+        <v>3795</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5">
-        <v>55.25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6">
-        <v>3795</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6">
         <v>5</v>
       </c>
     </row>

</xml_diff>